<commit_message>
chore: init project (gradle, ignore, readme, templates)
</commit_message>
<xml_diff>
--- a/funcionarios.xlsx
+++ b/funcionarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heito\OneDrive\Área de Trabalho\contraApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Microsoft\Desktop\ContraX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABDE3BD-CF75-4AD8-89A1-3518D1C86B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFD52EA-E31D-4C1A-A09E-B51AB82AE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Miguel Matias</t>
-  </si>
-  <si>
-    <t>miguel matias.pdf</t>
-  </si>
-  <si>
-    <t>Ramon</t>
-  </si>
-  <si>
-    <t>ramon.pdf</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nome</t>
   </si>
@@ -43,10 +31,28 @@
     <t>Arquivo</t>
   </si>
   <si>
-    <t>bella</t>
-  </si>
-  <si>
-    <t>bella.pdf</t>
+    <t>HEITOR MAMEDE</t>
+  </si>
+  <si>
+    <t>ROBERTA MOURA</t>
+  </si>
+  <si>
+    <t>IAGO JULIANO</t>
+  </si>
+  <si>
+    <t>CAUA SANTANA</t>
+  </si>
+  <si>
+    <t>HEITOR MAMEDE.pdf</t>
+  </si>
+  <si>
+    <t>ROBERTA MOURA.pdf</t>
+  </si>
+  <si>
+    <t>IAGO JULIANO.pdf</t>
+  </si>
+  <si>
+    <t>CAUA SANTANA.pdf</t>
   </si>
 </sst>
 </file>
@@ -149,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,9 +195,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +230,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,9 +282,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,59 +490,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>987999999</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>83993238060</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>8399999999</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>83987317588</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>9999999999</v>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>83991071312</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>83986901565</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>